<commit_message>
Added some more manual tests
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SynopticProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C9235-6335-4B72-BB3A-3D7EFEE5F3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BA14D7-1242-465E-83BB-F1A8B1885676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10071397-81EC-4882-A7EA-BCD71D56A078}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Test Number</t>
   </si>
@@ -51,49 +51,43 @@
     <t>Pass / Fail</t>
   </si>
   <si>
-    <t>I am given a list of all holidays that are in the "Active" Category</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Reply to every question except category with "No". Reply to Active or Lazy with "Active"</t>
-  </si>
-  <si>
-    <t>Reply to every question except category with "No". Reply to Active or Lazy with "Lazy"</t>
-  </si>
-  <si>
-    <t>I am given a list of all holidays that are in the "Lazy" Category</t>
-  </si>
-  <si>
-    <t>Reply "No" to every question except for Continent. Reply to Continent with "Asia"</t>
-  </si>
-  <si>
-    <t>Reply "No" to every question except for Continent. Reply to Continent with "Africa"</t>
-  </si>
-  <si>
-    <t>Reply "No" to every question except for Continent. Reply to Continent with "North America"</t>
-  </si>
-  <si>
-    <t>I am given a list of active holidays in African countries</t>
-  </si>
-  <si>
-    <t>I am given a list of active holidays in Asian countries</t>
-  </si>
-  <si>
-    <t>I am given a list of active holidays in North American countries</t>
-  </si>
-  <si>
-    <t>I am given a list of active holidays for £50 / Night or under.</t>
-  </si>
-  <si>
-    <t>Reply "No" to every question except for Continent, and Price Limit. Reply to Continent with "Europe", reply to Price Limit with "50"</t>
-  </si>
-  <si>
-    <t>Reply "No" to every question except for Price Limit. Reply to Price limit with "50"</t>
-  </si>
-  <si>
-    <t>I am give a list of active holidays in Europe for £50 / Night or under.</t>
+    <t>I fill every question with "no" or "either"</t>
+  </si>
+  <si>
+    <t>I am given a list of all holidays.</t>
+  </si>
+  <si>
+    <t>I fill every question with "no" except Category, which I say "Active" to</t>
+  </si>
+  <si>
+    <t>I am given a list of all "Active" holidays</t>
+  </si>
+  <si>
+    <t>I am given a list of all holidays in Asian countries.</t>
+  </si>
+  <si>
+    <t>I fill every question with "no" or "either", except for Upper Price Limit, which I say "50" to.</t>
+  </si>
+  <si>
+    <t>I am given a list of holidays at or under £50 / Night</t>
+  </si>
+  <si>
+    <t>I fill every question with "no" or "either", except for Location, which I say "city" to.</t>
+  </si>
+  <si>
+    <t>I fill every question with "no" or "either", except for Continent, which I say "Asia" to.</t>
+  </si>
+  <si>
+    <t>I am given a list of holidays in the City.</t>
+  </si>
+  <si>
+    <t>I fill every question with "no" or "either", except for TempRating which I say "mild" to.</t>
+  </si>
+  <si>
+    <t>I am given a list of holidays in Mild temperature areas.</t>
   </si>
 </sst>
 </file>
@@ -149,12 +143,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -164,7 +152,13 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -180,14 +174,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{126AC3FC-18B0-4F5D-873C-133982E80992}" name="Table1" displayName="Table1" ref="A1:E41" totalsRowShown="0" headerRowDxfId="1" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{126AC3FC-18B0-4F5D-873C-133982E80992}" name="Table1" displayName="Table1" ref="A1:E41" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E41" xr:uid="{126AC3FC-18B0-4F5D-873C-133982E80992}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1081231A-163F-444D-9765-529BCE39175C}" name="Test Number" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1081231A-163F-444D-9765-529BCE39175C}" name="Test Number" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{330A4732-53C8-483A-B057-26CCC69A21D3}" name="Test Description" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3BBC815E-3DAE-4A29-B9D9-AA8FF885D746}" name="Expected Outcome" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{C77784F6-1456-4BE2-AE14-066C7D267827}" name="Actual Outcome" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{AFF8074A-4584-47BD-B9FC-6848B42FB467}" name="Pass / Fail" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3BBC815E-3DAE-4A29-B9D9-AA8FF885D746}" name="Expected Outcome" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C77784F6-1456-4BE2-AE14-066C7D267827}" name="Actual Outcome" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{AFF8074A-4584-47BD-B9FC-6848B42FB467}" name="Pass / Fail" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863B9818-1FC2-4BE2-8969-C872E32BC830}">
-  <dimension ref="A1:HP41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="HP1" sqref="HP1:HP1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -524,16 +518,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -550,7 +544,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -558,16 +552,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -578,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -592,7 +586,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -601,7 +595,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -609,34 +603,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">

</xml_diff>

<commit_message>
did some more manual tests
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SynopticProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BA14D7-1242-465E-83BB-F1A8B1885676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C32D01-0A15-4475-BBBB-16134C48E3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10071397-81EC-4882-A7EA-BCD71D56A078}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10071397-81EC-4882-A7EA-BCD71D56A078}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tests" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Test Number</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>I am given a list of holidays in Mild temperature areas.</t>
+  </si>
+  <si>
+    <t>I fill every question with "no" or "either", except for StarRating which I say "3" to.</t>
+  </si>
+  <si>
+    <t>I am given a lsit of holidays that are 3 starts or higher.</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -619,10 +625,18 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">

</xml_diff>

<commit_message>
Thought I submitted all of this on friday lol
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SynopticProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D0256B-9ECE-4991-B3DD-D9702D9A72EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EBC364-78EB-4746-BD58-13A6D991D1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10071397-81EC-4882-A7EA-BCD71D56A078}"/>
   </bookViews>
@@ -523,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863B9818-1FC2-4BE2-8969-C872E32BC830}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="HQ6" sqref="HQ6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -945,13 +945,6 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>